<commit_message>
modified feature finished program v1 without debug
</commit_message>
<xml_diff>
--- a/feature.xlsx
+++ b/feature.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>特征清单</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -50,14 +50,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>商品类</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>平均单价</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>为每个中类分别训练一个学习器</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -94,11 +86,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>唯一性数据</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>总日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>节假日前</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>促销类</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>月份</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>唯一性数据</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -177,14 +181,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -495,130 +499,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D6" sqref="D6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="11" max="11" width="8.88671875" style="1"/>
+    <col min="1" max="3" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="K5" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="L5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>